<commit_message>
added more content + clarify the WFD source code
</commit_message>
<xml_diff>
--- a/paper/sac2017/summary_discover.xlsx
+++ b/paper/sac2017/summary_discover.xlsx
@@ -2382,8 +2382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="G201" sqref="G201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6238,7 +6238,18 @@
       <c r="C201">
         <v>1472677848965</v>
       </c>
-      <c r="I201" s="2"/>
+      <c r="G201">
+        <f>AVERAGE(G2:G200)</f>
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="H201">
+        <f>AVERAGE(H2:H200)</f>
+        <v>18.41</v>
+      </c>
+      <c r="I201">
+        <f>AVERAGE(I2:I200)</f>
+        <v>13.58</v>
+      </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
@@ -9263,7 +9274,7 @@
         <v>1473469350270</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I3:I66" si="0">H4-H3</f>
+        <f t="shared" ref="I4:I66" si="0">H4-H3</f>
         <v>9</v>
       </c>
     </row>
@@ -10799,7 +10810,7 @@
         <v>1473469368235</v>
       </c>
       <c r="I68" s="2">
-        <f t="shared" ref="I67:I130" si="2">H68-H67</f>
+        <f t="shared" ref="I68:I130" si="2">H68-H67</f>
         <v>9</v>
       </c>
     </row>
@@ -12335,7 +12346,7 @@
         <v>1473469382821</v>
       </c>
       <c r="I132" s="2">
-        <f t="shared" ref="I131:I194" si="4">H132-H131</f>
+        <f t="shared" ref="I132:I194" si="4">H132-H131</f>
         <v>14</v>
       </c>
     </row>
@@ -13871,7 +13882,7 @@
         <v>1473469399033</v>
       </c>
       <c r="I196" s="2">
-        <f t="shared" ref="I195:I258" si="6">H196-H195</f>
+        <f t="shared" ref="I196:I258" si="6">H196-H195</f>
         <v>16</v>
       </c>
     </row>
@@ -15363,7 +15374,7 @@
         <v>1473469416093</v>
       </c>
       <c r="I260" s="2">
-        <f t="shared" ref="I259:I322" si="7">H260-H259</f>
+        <f t="shared" ref="I260:I322" si="7">H260-H259</f>
         <v>11</v>
       </c>
     </row>
@@ -16195,7 +16206,7 @@
         <v>1473469432386</v>
       </c>
       <c r="I324" s="2">
-        <f t="shared" ref="I323:I386" si="8">H324-H323</f>
+        <f t="shared" ref="I324:I386" si="8">H324-H323</f>
         <v>15</v>
       </c>
     </row>
@@ -17027,7 +17038,7 @@
         <v>1473469453160</v>
       </c>
       <c r="I388" s="2">
-        <f t="shared" ref="I387:I410" si="9">H388-H387</f>
+        <f t="shared" ref="I388:I410" si="9">H388-H387</f>
         <v>15</v>
       </c>
     </row>

</xml_diff>